<commit_message>
updated payments option branch
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA348.xlsx
+++ b/src/test/resources/data/jdgroupTA348.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D344F5EF-AE2F-4953-ADAC-CEEE84E9CD3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9885EE-DB35-497D-8373-47EB01F78EC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -2145,13 +2145,13 @@
     <t>JBL Tune600 Black</t>
   </si>
   <si>
-    <t>Types_of_Payments</t>
-  </si>
-  <si>
-    <t>Cash Deposits</t>
-  </si>
-  <si>
     <t>CartTotal</t>
+  </si>
+  <si>
+    <t>PaymentOptions</t>
+  </si>
+  <si>
+    <t>Credit Card (Processed By PayU)|Visa Checkout|EFT Pro (Processed By PayU)|Masterpass|Pay with PayGate|Cash Deposits</t>
   </si>
 </sst>
 </file>
@@ -2329,7 +2329,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2516,6 +2516,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3431,11 +3432,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H61" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B77" sqref="B77"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A77:XFD77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -8115,15 +8116,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D99E3A93-DE6D-4C3C-A63A-888395F95841}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="104.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="35" customFormat="1">
@@ -8136,8 +8137,8 @@
       <c r="C1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>668</v>
+      <c r="D1" s="86" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -8151,15 +8152,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{19F8F523-1467-419E-82C1-CE3E37C8B9FF}">
-      <formula1>"Credit Card (Processed By PayU),Visa Checkout,EFT Pro (Processed By PayU),Masterpass,Pay with PayGate,Cash Deposits"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -18820,7 +18816,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="42" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>